<commit_message>
Revision catalogo de producto
</commit_message>
<xml_diff>
--- a/Organización/Catalogo/catalogo_productos.xlsx
+++ b/Organización/Catalogo/catalogo_productos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="164">
   <si>
     <t>Concepto</t>
   </si>
@@ -431,9 +431,6 @@
     <t>Paquete de 5 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota</t>
   </si>
   <si>
-    <t>0min</t>
-  </si>
-  <si>
     <t>Paquete de 2 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota (Incluye 2 horas gratis por ser cliente distinguido)</t>
   </si>
   <si>
@@ -452,16 +449,7 @@
     <t>Servicio de Implementación de los Sistemas de Contpaq i® Servicio Vía Remota por hora</t>
   </si>
   <si>
-    <t>Paquete de días para capacitación en los Sistemas easy Retail Admin y Contpaq i®, Servicio Presencial</t>
-  </si>
-  <si>
-    <t>Servicio de Instalación y activación de los usuarios adicionales en red de Contpaqi Servicio Vía Remota</t>
-  </si>
-  <si>
     <t>Interfaz entre los Productos Contpaq i®</t>
-  </si>
-  <si>
-    <t>Precapacitación para la captura de información para la interfaz Servicio Vía Remota</t>
   </si>
   <si>
     <t>Join Data</t>
@@ -720,17 +708,24 @@
     <t>USD</t>
   </si>
   <si>
-    <t>Thinstuff</t>
+    <t>2 semanas</t>
+  </si>
+  <si>
+    <t>240 min</t>
+  </si>
+  <si>
+    <t>120 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-80A]#,##0.00;[Red]\-[$$-80A]#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -923,7 +918,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1017,6 +1012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1388,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F136" sqref="A136:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,13 +3703,13 @@
         <v>129</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D128" s="17">
-        <v>0</v>
+        <v>2625</v>
       </c>
       <c r="E128" s="17">
         <v>2625</v>
@@ -3724,7 +3720,7 @@
     </row>
     <row r="129" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B129" s="16" t="s">
         <v>95</v>
@@ -3733,7 +3729,7 @@
         <v>95</v>
       </c>
       <c r="D129" s="17">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="E129" s="17">
         <v>1100</v>
@@ -3746,7 +3742,7 @@
     </row>
     <row r="130" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B130" s="16" t="s">
         <v>16</v>
@@ -3755,7 +3751,7 @@
         <v>16</v>
       </c>
       <c r="D130" s="17">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="E130" s="17">
         <v>1100</v>
@@ -3768,16 +3764,16 @@
     </row>
     <row r="131" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="C131" s="16" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="D131" s="17">
-        <v>0</v>
+        <v>3250</v>
       </c>
       <c r="E131" s="17">
         <v>0</v>
@@ -3790,16 +3786,16 @@
     </row>
     <row r="132" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="C132" s="16" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="D132" s="17">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E132" s="17">
         <v>0</v>
@@ -3812,16 +3808,16 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="C133" s="16" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="D133" s="17">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E133" s="17">
         <v>0</v>
@@ -3834,16 +3830,16 @@
     </row>
     <row r="134" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="D134" s="17">
-        <v>0</v>
+        <v>550</v>
       </c>
       <c r="E134" s="17">
         <v>550</v>
@@ -3854,18 +3850,18 @@
       <c r="I134" s="18"/>
       <c r="J134" s="18"/>
     </row>
-    <row r="135" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="C135" s="16" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="D135" s="17">
-        <v>0</v>
+        <v>1890</v>
       </c>
       <c r="E135" s="17">
         <v>0</v>
@@ -3876,261 +3872,274 @@
       <c r="I135" s="18"/>
       <c r="J135" s="18"/>
     </row>
-    <row r="136" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B136" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C136" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D136" s="17">
-        <v>0</v>
-      </c>
-      <c r="E136" s="17">
-        <v>0</v>
-      </c>
-      <c r="F136" s="18"/>
-      <c r="G136" s="18"/>
-      <c r="H136" s="18"/>
-      <c r="I136" s="18"/>
-      <c r="J136" s="18"/>
+    <row r="136" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B137" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C137" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D137" s="17">
-        <v>0</v>
-      </c>
-      <c r="E137" s="17">
-        <v>0</v>
-      </c>
-      <c r="F137" s="18"/>
-      <c r="G137" s="18"/>
-      <c r="H137" s="18"/>
-      <c r="I137" s="18"/>
-      <c r="J137" s="18"/>
-    </row>
-    <row r="138" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B138" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C138" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D138" s="17">
-        <v>0</v>
-      </c>
-      <c r="E138" s="17">
-        <v>0</v>
-      </c>
-      <c r="F138" s="18"/>
-      <c r="G138" s="18"/>
-      <c r="H138" s="18"/>
-      <c r="I138" s="18"/>
-      <c r="J138" s="18"/>
-    </row>
-    <row r="139" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
-      <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
+    <row r="140" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B140" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C140" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D140" s="39">
+        <v>8400</v>
+      </c>
+      <c r="E140" s="20"/>
+    </row>
+    <row r="141" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A141" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C141" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D141" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E141" s="26" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
-    </row>
-    <row r="143" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" s="16" t="s">
+      <c r="A142" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B142" s="22">
+        <v>39.9</v>
+      </c>
+      <c r="C142" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D142" s="33">
+        <v>18.05</v>
+      </c>
+      <c r="E142" s="27">
+        <f>B142*1.16*D142*1.5</f>
+        <v>1253.1392999999998</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B143" s="19"/>
-      <c r="C143" s="19"/>
-      <c r="D143" s="20"/>
-      <c r="E143" s="20"/>
+      <c r="B143" s="22">
+        <v>99</v>
+      </c>
+      <c r="C143" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D143" s="33"/>
+      <c r="E143" s="27">
+        <f>B143*1.16*D142*1.5</f>
+        <v>3109.2930000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B144" s="22">
+        <v>139</v>
+      </c>
+      <c r="C144" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D144" s="33"/>
+      <c r="E144" s="27">
+        <f>B144*1.16*D142*1.5</f>
+        <v>4365.5729999999994</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B145" s="22">
+        <v>199</v>
+      </c>
+      <c r="C145" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D145" s="33"/>
+      <c r="E145" s="27">
+        <f>B145*1.16*D142*1.5</f>
+        <v>6249.9929999999986</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B146" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A148" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B148" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="C148" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="D148" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="E148" s="26" t="s">
+      <c r="A146" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B146" s="22">
+        <v>299</v>
+      </c>
+      <c r="C146" s="32" t="s">
         <v>160</v>
       </c>
+      <c r="D146" s="33"/>
+      <c r="E146" s="27">
+        <f>B146*1.16*D142*1.5</f>
+        <v>9390.6929999999993</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" s="22"/>
+      <c r="C147" s="22"/>
+      <c r="D147" s="33"/>
+      <c r="E147" s="28"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" s="34">
+        <v>242</v>
+      </c>
+      <c r="C148" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D148" s="33"/>
+      <c r="E148" s="29">
+        <f>B148*1.16*D142*1.3</f>
+        <v>6587.0948000000008</v>
+      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B149" s="22">
-        <v>39.9</v>
-      </c>
-      <c r="C149" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D149" s="33">
-        <v>18.05</v>
-      </c>
-      <c r="E149" s="27">
-        <f>B149*1.16*D149*1.5</f>
-        <v>1253.1392999999998</v>
-      </c>
+      <c r="A149" s="24"/>
+      <c r="B149" s="34"/>
+      <c r="C149" s="35"/>
+      <c r="D149" s="33"/>
+      <c r="E149" s="29"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B150" s="22">
-        <v>99</v>
-      </c>
-      <c r="C150" s="32" t="s">
-        <v>164</v>
+      <c r="A150" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B150" s="34">
+        <v>290</v>
+      </c>
+      <c r="C150" s="24" t="s">
+        <v>160</v>
       </c>
       <c r="D150" s="33"/>
-      <c r="E150" s="27">
-        <f>B150*1.16*D149*1.5</f>
-        <v>3109.2930000000001</v>
+      <c r="E150" s="30">
+        <f>B150*1.16*D142*1.3</f>
+        <v>7893.6259999999993</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="B151" s="22">
-        <v>139</v>
-      </c>
-      <c r="C151" s="32" t="s">
-        <v>164</v>
-      </c>
+      <c r="A151" s="24"/>
+      <c r="B151" s="34"/>
+      <c r="C151" s="24"/>
       <c r="D151" s="33"/>
-      <c r="E151" s="27">
-        <f>B151*1.16*D149*1.5</f>
-        <v>4365.5729999999994</v>
-      </c>
+      <c r="E151" s="30"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="B152" s="22">
-        <v>199</v>
-      </c>
-      <c r="C152" s="32" t="s">
-        <v>164</v>
+      <c r="A152" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B152" s="36">
+        <v>370</v>
+      </c>
+      <c r="C152" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="D152" s="33"/>
-      <c r="E152" s="27">
-        <f>B152*1.16*D149*1.5</f>
-        <v>6249.9929999999986</v>
+      <c r="E152" s="29">
+        <f>B152*1.16*D142*1.3</f>
+        <v>10071.178000000002</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B153" s="22">
-        <v>299</v>
-      </c>
-      <c r="C153" s="32" t="s">
-        <v>164</v>
-      </c>
+      <c r="A153" s="24"/>
+      <c r="B153" s="36"/>
+      <c r="C153" s="35"/>
       <c r="D153" s="33"/>
-      <c r="E153" s="27">
-        <f>B153*1.16*D149*1.5</f>
-        <v>9390.6929999999993</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="23" t="s">
+      <c r="E153" s="29"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B154" s="22"/>
-      <c r="C154" s="22"/>
+      <c r="B154" s="34">
+        <v>530</v>
+      </c>
+      <c r="C154" s="24" t="s">
+        <v>160</v>
+      </c>
       <c r="D154" s="33"/>
-      <c r="E154" s="28"/>
+      <c r="E154" s="29">
+        <f>B154*1.16*D142*1.3</f>
+        <v>14426.281999999999</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="24" t="s">
+      <c r="A155" s="24"/>
+      <c r="B155" s="34"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="33"/>
+      <c r="E155" s="29"/>
+    </row>
+    <row r="156" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="B155" s="34">
-        <v>242</v>
-      </c>
-      <c r="C155" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="D155" s="33"/>
-      <c r="E155" s="29">
-        <f>B155*1.16*D149*1.3</f>
-        <v>6587.0948000000008</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="24"/>
-      <c r="B156" s="34"/>
-      <c r="C156" s="35"/>
+      <c r="B156" s="37"/>
+      <c r="C156" s="37"/>
       <c r="D156" s="33"/>
-      <c r="E156" s="29"/>
+      <c r="E156" s="28"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="24" t="s">
         <v>152</v>
       </c>
       <c r="B157" s="34">
-        <v>290</v>
+        <v>418</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D157" s="33"/>
-      <c r="E157" s="30">
-        <f>B157*1.16*D149*1.3</f>
-        <v>7893.6259999999993</v>
+      <c r="E157" s="29">
+        <f>B157*1.16*D142*1.3</f>
+        <v>11377.709199999999</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,194 +4147,116 @@
       <c r="B158" s="34"/>
       <c r="C158" s="24"/>
       <c r="D158" s="33"/>
-      <c r="E158" s="30"/>
+      <c r="E158" s="29"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="24" t="s">
+      <c r="A159" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B159" s="36">
-        <v>370</v>
-      </c>
-      <c r="C159" s="35" t="s">
-        <v>164</v>
+      <c r="B159" s="38">
+        <v>497</v>
+      </c>
+      <c r="C159" s="25" t="s">
+        <v>160</v>
       </c>
       <c r="D159" s="33"/>
       <c r="E159" s="29">
-        <f>B159*1.16*D149*1.3</f>
-        <v>10071.178000000002</v>
+        <f>B159*1.16*D142*1.3</f>
+        <v>13528.041800000001</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="24"/>
-      <c r="B160" s="36"/>
-      <c r="C160" s="35"/>
+      <c r="A160" s="25"/>
+      <c r="B160" s="38"/>
+      <c r="C160" s="25"/>
       <c r="D160" s="33"/>
       <c r="E160" s="29"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="24" t="s">
+      <c r="A161" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B161" s="34">
-        <v>530</v>
-      </c>
-      <c r="C161" s="24" t="s">
-        <v>164</v>
+      <c r="B161" s="38">
+        <v>649</v>
+      </c>
+      <c r="C161" s="25" t="s">
+        <v>160</v>
       </c>
       <c r="D161" s="33"/>
       <c r="E161" s="29">
-        <f>B161*1.16*D149*1.3</f>
-        <v>14426.281999999999</v>
+        <f>B161*1.16*D142*1.3</f>
+        <v>17665.390599999999</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="24"/>
-      <c r="B162" s="34"/>
-      <c r="C162" s="24"/>
+      <c r="A162" s="25"/>
+      <c r="B162" s="38"/>
+      <c r="C162" s="25"/>
       <c r="D162" s="33"/>
       <c r="E162" s="29"/>
     </row>
-    <row r="163" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="23" t="s">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B163" s="37"/>
-      <c r="C163" s="37"/>
+      <c r="B163" s="34">
+        <v>913</v>
+      </c>
+      <c r="C163" s="24" t="s">
+        <v>160</v>
+      </c>
       <c r="D163" s="33"/>
-      <c r="E163" s="28"/>
+      <c r="E163" s="29">
+        <f>B163*1.16*D142*1.3</f>
+        <v>24851.3122</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B164" s="34">
-        <v>418</v>
-      </c>
-      <c r="C164" s="24" t="s">
-        <v>164</v>
-      </c>
+      <c r="A164" s="24"/>
+      <c r="B164" s="34"/>
+      <c r="C164" s="24"/>
       <c r="D164" s="33"/>
-      <c r="E164" s="29">
-        <f>B164*1.16*D149*1.3</f>
-        <v>11377.709199999999</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="24"/>
-      <c r="B165" s="34"/>
-      <c r="C165" s="24"/>
-      <c r="D165" s="33"/>
-      <c r="E165" s="29"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B166" s="38">
-        <v>497</v>
-      </c>
-      <c r="C166" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="D166" s="33"/>
-      <c r="E166" s="29">
-        <f>B166*1.16*D149*1.3</f>
-        <v>13528.041800000001</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="25"/>
-      <c r="B167" s="38"/>
-      <c r="C167" s="25"/>
-      <c r="D167" s="33"/>
-      <c r="E167" s="29"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B168" s="38">
-        <v>649</v>
-      </c>
-      <c r="C168" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="D168" s="33"/>
-      <c r="E168" s="29">
-        <f>B168*1.16*D149*1.3</f>
-        <v>17665.390599999999</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="25"/>
-      <c r="B169" s="38"/>
-      <c r="C169" s="25"/>
-      <c r="D169" s="33"/>
-      <c r="E169" s="29"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B170" s="34">
-        <v>913</v>
-      </c>
-      <c r="C170" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D170" s="33"/>
-      <c r="E170" s="29">
-        <f>B170*1.16*D149*1.3</f>
-        <v>24851.3122</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="24"/>
-      <c r="B171" s="34"/>
-      <c r="C171" s="24"/>
-      <c r="D171" s="33"/>
-      <c r="E171" s="29"/>
+      <c r="E164" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B168:B169"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="E168:E169"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="B170:B171"/>
-    <mergeCell ref="C170:C171"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="E164:E165"/>
-    <mergeCell ref="B166:B167"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="E166:E167"/>
-    <mergeCell ref="D149:D171"/>
-    <mergeCell ref="E155:E156"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="C161:C162"/>
+    <mergeCell ref="E161:E162"/>
+    <mergeCell ref="A163:A164"/>
+    <mergeCell ref="B163:B164"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="C157:C158"/>
     <mergeCell ref="E157:E158"/>
     <mergeCell ref="B159:B160"/>
     <mergeCell ref="C159:C160"/>
     <mergeCell ref="E159:E160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="C161:C162"/>
-    <mergeCell ref="B155:B156"/>
-    <mergeCell ref="C155:C156"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="E161:E162"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="D142:D164"/>
+    <mergeCell ref="E148:E149"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="C152:C153"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A159:A160"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="A152:A153"/>
     <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A159:A160"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="A155:A156"/>
-    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="A150:A151"/>
     <mergeCell ref="A2:E5"/>
     <mergeCell ref="A89:E91"/>
     <mergeCell ref="A124:E127"/>
-    <mergeCell ref="A139:E142"/>
+    <mergeCell ref="A136:E139"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>